<commit_message>
SD-93955 - CCRU - MT POS Update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - OTH.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - OTH.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -650,7 +651,7 @@
     <t xml:space="preserve">Активация Комбо</t>
   </si>
   <si>
-    <t xml:space="preserve">number of atomic KPI Passed on the same scene</t>
+    <t xml:space="preserve">number of atomic KPI Passed</t>
   </si>
   <si>
     <t xml:space="preserve">Menu Board, Cash Zone</t>
@@ -1056,52 +1057,52 @@
   <dimension ref="A1:AL55"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3036437246964"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8259109311741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6761133603239"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4898785425101"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5627530364372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="70.5182186234818"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="78.834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.0404858299595"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7449392712551"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.45344129554656"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.6963562753036"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="102.412955465587"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.1214574898785"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.4089068825911"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.2955465587045"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="71.1255060728745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="79.4817813765182"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="103.368421052632"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.6315789473684"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.246963562753"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.4939271255061"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.24696356275304"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.9392712550607"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.8502024291498"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.3441295546559"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="23.3643724696356"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.4817813765182"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.9068825910931"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.417004048583"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.7449392712551"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.6963562753036"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.8461538461538"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3522267206478"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="62.5506072874494"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="22.5182186234818"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7813765182186"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.6720647773279"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.7125506072874"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="63.0931174089069"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.11336032388664"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1457489878543"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.62753036437247"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.74898785425101"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Revert "SD-93955 - CCRU - MT POS Update"
This reverts commit 48bc0a4
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - OTH.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC Canteen - OTH.xlsx
@@ -14,7 +14,6 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Canteen!$A$1:$AL$55</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -651,7 +650,7 @@
     <t xml:space="preserve">Активация Комбо</t>
   </si>
   <si>
-    <t xml:space="preserve">number of atomic KPI Passed</t>
+    <t xml:space="preserve">number of atomic KPI Passed on the same scene</t>
   </si>
   <si>
     <t xml:space="preserve">Menu Board, Cash Zone</t>
@@ -1057,52 +1056,52 @@
   <dimension ref="A1:AL55"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
+      <selection pane="bottomLeft" activeCell="H15" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.45"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="71.1255060728745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="79.4817813765182"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.3522267206478"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="103.368421052632"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.6315789473684"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3036437246964"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8259109311741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.6761133603239"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4898785425101"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="70.5182186234818"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="78.834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.0404858299595"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.7449392712551"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.45344129554656"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.6963562753036"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="14.2024291497976"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="102.412955465587"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="57.1214574898785"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.4089068825911"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="19.2955465587045"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="1" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.2834008097166"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.4939271255061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="23.4574898785425"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.6720647773279"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.9230769230769"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="63.0931174089069"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="22.7085020242915"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="7.24696356275304"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="14.7125506072875"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="17.9392712550607"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="22.3441295546559"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="23.3643724696356"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="20.4817813765182"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.9068825910931"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="26.417004048583"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="16.7449392712551"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="13.6963562753036"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="12.8461538461538"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="13.3522267206478"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="62.5506072874494"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="22.5182186234818"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="1" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.11336032388664"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="11.1457489878543"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="9.62753036437247"/>
+    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>